<commit_message>
Update medfind server - Update pharmacies with the working hours column
</commit_message>
<xml_diff>
--- a/files/farmacii.xlsx
+++ b/files/farmacii.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="farmacii" sheetId="1" r:id="rId1"/>
+    <sheet name="Coordonate Farmacii HN" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="418">
   <si>
     <t>1, HELP NET FARMA - TIMISOARA</t>
   </si>
@@ -38,6 +38,9 @@
     <t>Str. Gh. Lazar, nr.30</t>
   </si>
   <si>
+    <t>NON STOP</t>
+  </si>
+  <si>
     <t>2, HELP NET FARMA - CAMIL RESSU</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
     <t>Bd. Camil Ressu, nr.12</t>
   </si>
   <si>
+    <t>9 :00- 21:00</t>
+  </si>
+  <si>
     <t>3, HELP NET FARMA - GARA DE NORD</t>
   </si>
   <si>
@@ -1121,15 +1127,6 @@
     <t>Str. Aleea Spitalului nr. 18</t>
   </si>
   <si>
-    <t>126, HELP NET FARMA - TIMISOARA 10</t>
-  </si>
-  <si>
-    <t>Calea Sagului Nr. 22</t>
-  </si>
-  <si>
-    <t>tbd</t>
-  </si>
-  <si>
     <t>127, HELP NET FARMA - IULIU MANIU 78-92 2</t>
   </si>
   <si>
@@ -1241,6 +1238,9 @@
     <t>Sos. Alexandriei, Nr. 152, Sector 5, Bucuresti ( zona Autogara Rahova)</t>
   </si>
   <si>
+    <t>144, GALATI</t>
+  </si>
+  <si>
     <t>In galeria comerciala a complexului Kaufland, str. Braila nr 144</t>
   </si>
   <si>
@@ -1262,16 +1262,22 @@
     <t>B-dul Ion Mihalache , nr. 201</t>
   </si>
   <si>
+    <t>148, HELP NET SNAGOV</t>
+  </si>
+  <si>
     <t>Sos. Ghermanesti, nr.59, sat. Ghermanesti</t>
   </si>
   <si>
     <t>SNAGOV</t>
   </si>
   <si>
-    <t>148, HELP NET SNAGOV</t>
-  </si>
-  <si>
-    <t>144, HELP NET GALATI</t>
+    <t>1000, HELP NET FARMA S.A. - SEDIU</t>
+  </si>
+  <si>
+    <t>Sediu HelpNet</t>
+  </si>
+  <si>
+    <t>Str. Ing George Consantinescu, Nr. 2-4</t>
   </si>
 </sst>
 </file>
@@ -1586,20 +1592,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F147"/>
+  <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
-    <col min="2" max="2" width="67.83203125" customWidth="1"/>
-    <col min="4" max="4" width="27.5" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1618,19 +1617,22 @@
       <c r="F1">
         <v>21.218022999999999</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>44.418328000000002</v>
@@ -1638,19 +1640,22 @@
       <c r="F2">
         <v>26.142759000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>44.444952000000001</v>
@@ -1658,19 +1663,22 @@
       <c r="F3">
         <v>26.074269000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>44.440365999999997</v>
@@ -1678,19 +1686,22 @@
       <c r="F4">
         <v>26.133980999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>44.414625999999998</v>
@@ -1698,19 +1709,22 @@
       <c r="F5">
         <v>26.174358999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>44.438066999999997</v>
@@ -1718,19 +1732,22 @@
       <c r="F6">
         <v>26.138818000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E7">
         <v>44.433847999999998</v>
@@ -1738,19 +1755,22 @@
       <c r="F7">
         <v>26.019860000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E8">
         <v>44.418968</v>
@@ -1758,19 +1778,22 @@
       <c r="F8">
         <v>26.140345</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E9">
         <v>44.437998999999998</v>
@@ -1778,19 +1801,22 @@
       <c r="F9">
         <v>26.158463000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E10">
         <v>44.434699000000002</v>
@@ -1798,19 +1824,22 @@
       <c r="F10">
         <v>26.029105999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E11">
         <v>44.453736999999997</v>
@@ -1818,19 +1847,22 @@
       <c r="F11">
         <v>26.050595999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E12">
         <v>44.452724000000003</v>
@@ -1838,19 +1870,22 @@
       <c r="F12">
         <v>26.098555000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E13">
         <v>44.444141999999999</v>
@@ -1858,19 +1893,22 @@
       <c r="F13">
         <v>26.119586000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E14">
         <v>44.427613999999998</v>
@@ -1878,19 +1916,22 @@
       <c r="F14">
         <v>26.100777000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E15">
         <v>44.460303000000003</v>
@@ -1898,19 +1939,22 @@
       <c r="F15">
         <v>26.075462000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E16">
         <v>44.423316999999997</v>
@@ -1918,19 +1962,22 @@
       <c r="F16">
         <v>26.071905999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E17">
         <v>44.941369999999999</v>
@@ -1938,19 +1985,22 @@
       <c r="F17">
         <v>26.020885</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E18">
         <v>44.441850000000002</v>
@@ -1958,19 +2008,22 @@
       <c r="F18">
         <v>26.138103999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E19">
         <v>44.419426000000001</v>
@@ -1978,19 +2031,22 @@
       <c r="F19">
         <v>26.048089999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E20">
         <v>44.427194</v>
@@ -1998,19 +2054,22 @@
       <c r="F20">
         <v>26.137715</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E21">
         <v>45.794848000000002</v>
@@ -2018,19 +2077,22 @@
       <c r="F21">
         <v>20.723868299999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E22">
         <v>44.199826899999998</v>
@@ -2038,19 +2100,22 @@
       <c r="F22">
         <v>28.6274695</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E23">
         <v>46.070044600000003</v>
@@ -2058,19 +2123,22 @@
       <c r="F23">
         <v>20.629836000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E24">
         <v>46.181818100000001</v>
@@ -2078,19 +2146,22 @@
       <c r="F24">
         <v>21.317266100000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E25">
         <v>44.435875000000003</v>
@@ -2098,19 +2169,22 @@
       <c r="F25">
         <v>26.104968</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E26">
         <v>44.411040999999997</v>
@@ -2118,19 +2192,22 @@
       <c r="F26">
         <v>26.071179000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E27">
         <v>44.463020999999998</v>
@@ -2138,19 +2215,22 @@
       <c r="F27">
         <v>26.131056999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E28">
         <v>45.102862999999999</v>
@@ -2158,19 +2238,22 @@
       <c r="F28">
         <v>24.366403999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E29">
         <v>45.642636600000003</v>
@@ -2178,19 +2261,22 @@
       <c r="F29">
         <v>25.588733000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" t="s">
         <v>91</v>
       </c>
-      <c r="C30" t="s">
-        <v>89</v>
-      </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E30">
         <v>45.644553000000002</v>
@@ -2198,19 +2284,22 @@
       <c r="F30">
         <v>25.591963</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E31">
         <v>44.857387299999999</v>
@@ -2218,19 +2307,22 @@
       <c r="F31">
         <v>24.8743503</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E32">
         <v>44.452323999999997</v>
@@ -2238,19 +2330,22 @@
       <c r="F32">
         <v>26.071999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D33" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E33">
         <v>44.842406199999999</v>
@@ -2258,19 +2353,22 @@
       <c r="F33">
         <v>24.881284999999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E34">
         <v>44.466073000000002</v>
@@ -2278,19 +2376,22 @@
       <c r="F34">
         <v>26.067288000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E35">
         <v>44.461759000000001</v>
@@ -2298,19 +2399,22 @@
       <c r="F35">
         <v>26.094943000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E36">
         <v>45.758309099999998</v>
@@ -2318,19 +2422,22 @@
       <c r="F36">
         <v>21.2260092</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B37" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E37">
         <v>44.948872999999999</v>
@@ -2338,19 +2445,22 @@
       <c r="F37">
         <v>26.007830999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E38">
         <v>44.425972000000002</v>
@@ -2358,19 +2468,22 @@
       <c r="F38">
         <v>26.148161000000002</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E39">
         <v>46.043650999999997</v>
@@ -2378,19 +2491,22 @@
       <c r="F39">
         <v>20.477035000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C40" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E40">
         <v>46.070371000000002</v>
@@ -2398,19 +2514,22 @@
       <c r="F40">
         <v>23.576908</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" t="s">
         <v>125</v>
       </c>
-      <c r="C41" t="s">
-        <v>123</v>
-      </c>
       <c r="D41" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E41">
         <v>46.0705721</v>
@@ -2418,19 +2537,22 @@
       <c r="F41">
         <v>23.558090400000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B42" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E42">
         <v>44.414706000000002</v>
@@ -2438,19 +2560,22 @@
       <c r="F42">
         <v>26.107213000000002</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B43" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E43">
         <v>44.421385000000001</v>
@@ -2458,19 +2583,22 @@
       <c r="F43">
         <v>26.064845999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C44" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D44" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E44">
         <v>45.427604299999999</v>
@@ -2478,19 +2606,22 @@
       <c r="F44">
         <v>28.029478900000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B45" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E45">
         <v>44.427210000000002</v>
@@ -2498,19 +2629,22 @@
       <c r="F45">
         <v>26.066292000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B46" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E46">
         <v>44.422725999999997</v>
@@ -2518,19 +2652,22 @@
       <c r="F46">
         <v>26.034815999999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B47" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E47">
         <v>44.434350999999999</v>
@@ -2538,19 +2675,22 @@
       <c r="F47">
         <v>26.019072000000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B48" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E48">
         <v>44.460168000000003</v>
@@ -2558,19 +2698,22 @@
       <c r="F48">
         <v>26.099875000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B49" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E49">
         <v>44.462114</v>
@@ -2578,19 +2721,22 @@
       <c r="F49">
         <v>26.072040000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B50" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E50">
         <v>44.425083000000001</v>
@@ -2598,19 +2744,22 @@
       <c r="F50">
         <v>26.165904999999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D51" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E51">
         <v>44.414600999999998</v>
@@ -2618,19 +2767,22 @@
       <c r="F51">
         <v>26.104959999999998</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B52" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E52">
         <v>44.444175999999999</v>
@@ -2638,19 +2790,22 @@
       <c r="F52">
         <v>26.096990999999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B53" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E53">
         <v>44.461148999999999</v>
@@ -2658,19 +2813,22 @@
       <c r="F53">
         <v>26.094436000000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B54" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C54" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D54" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E54">
         <v>43.908444000000003</v>
@@ -2678,19 +2836,22 @@
       <c r="F54">
         <v>25.971115999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B55" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E55">
         <v>45.749707800000003</v>
@@ -2698,19 +2859,22 @@
       <c r="F55">
         <v>21.207920000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B56" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E56">
         <v>44.433197</v>
@@ -2718,19 +2882,22 @@
       <c r="F56">
         <v>26.120038999999998</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B57" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C57" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D57" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E57">
         <v>46.774342099999998</v>
@@ -2738,19 +2905,22 @@
       <c r="F57">
         <v>23.592142899999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B58" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D58" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E58">
         <v>44.452336000000003</v>
@@ -2758,19 +2928,22 @@
       <c r="F58">
         <v>26.081724999999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B59" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C59" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D59" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E59">
         <v>44.940671000000002</v>
@@ -2778,19 +2951,22 @@
       <c r="F59">
         <v>26.024774000000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B60" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C60" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D60" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E60">
         <v>47.7915086</v>
@@ -2798,19 +2974,22 @@
       <c r="F60">
         <v>22.873615699999998</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B61" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C61" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D61" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E61">
         <v>44.562461900000002</v>
@@ -2818,19 +2997,22 @@
       <c r="F61">
         <v>27.3761616</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B62" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C62" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D62" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E62">
         <v>45.955598299999998</v>
@@ -2838,19 +3020,22 @@
       <c r="F62">
         <v>23.577897499999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B63" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C63" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D63" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E63">
         <v>44.560994000000001</v>
@@ -2858,19 +3043,22 @@
       <c r="F63">
         <v>27.347062999999999</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B64" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C64" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D64" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E64">
         <v>47.791797000000003</v>
@@ -2878,19 +3066,22 @@
       <c r="F64">
         <v>22.873833099999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B65" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C65" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D65" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E65">
         <v>45.686609799999999</v>
@@ -2898,19 +3089,22 @@
       <c r="F65">
         <v>21.9061089</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B66" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C66" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D66" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E66">
         <v>45.8824015</v>
@@ -2918,19 +3112,22 @@
       <c r="F66">
         <v>22.904662900000002</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B67" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C67" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D67" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E67">
         <v>45.6425755</v>
@@ -2938,19 +3135,22 @@
       <c r="F67">
         <v>25.591038399999999</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B68" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C68" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D68" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E68">
         <v>46.181379</v>
@@ -2958,19 +3158,22 @@
       <c r="F68">
         <v>21.309062999999998</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B69" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C69" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D69" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E69">
         <v>47.6514904</v>
@@ -2978,19 +3181,22 @@
       <c r="F69">
         <v>23.569611999999999</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B70" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D70" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E70">
         <v>44.459257999999998</v>
@@ -2998,19 +3204,22 @@
       <c r="F70">
         <v>26.127396000000001</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B71" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D71" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E71">
         <v>44.433540000000001</v>
@@ -3018,19 +3227,22 @@
       <c r="F71">
         <v>26.036090000000002</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B72" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C72" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D72" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E72">
         <v>45.865007499999997</v>
@@ -3038,19 +3250,22 @@
       <c r="F72">
         <v>25.787200800000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B73" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C73" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D73" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E73">
         <v>44.483987999999997</v>
@@ -3058,19 +3273,22 @@
       <c r="F73">
         <v>26.096625</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B74" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D74" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E74">
         <v>44.416189000000003</v>
@@ -3078,19 +3296,22 @@
       <c r="F74">
         <v>26.176217999999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B75" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C75" t="s">
         <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E75">
         <v>45.703533999999998</v>
@@ -3098,19 +3319,22 @@
       <c r="F75">
         <v>21.190546000000001</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B76" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D76" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E76">
         <v>44.486930999999998</v>
@@ -3118,19 +3342,22 @@
       <c r="F76">
         <v>26.037979</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B77" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D77" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E77">
         <v>44.393357000000002</v>
@@ -3138,19 +3365,22 @@
       <c r="F77">
         <v>26.109500000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B78" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C78" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D78" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E78">
         <v>47.170394100000003</v>
@@ -3158,19 +3388,22 @@
       <c r="F78">
         <v>27.564361300000002</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>236</v>
+      </c>
+      <c r="B79" t="s">
+        <v>237</v>
+      </c>
+      <c r="C79" t="s">
         <v>234</v>
       </c>
-      <c r="B79" t="s">
-        <v>235</v>
-      </c>
-      <c r="C79" t="s">
-        <v>232</v>
-      </c>
       <c r="D79" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E79">
         <v>47.163700599999999</v>
@@ -3178,19 +3411,22 @@
       <c r="F79">
         <v>27.591467699999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B80" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C80" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D80" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E80">
         <v>44.203690100000003</v>
@@ -3198,19 +3434,22 @@
       <c r="F80">
         <v>28.6486163</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B81" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C81" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D81" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E81">
         <v>44.438642000000002</v>
@@ -3218,19 +3457,22 @@
       <c r="F81">
         <v>26.104002000000001</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B82" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C82" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D82" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E82">
         <v>45.6582857</v>
@@ -3238,19 +3480,22 @@
       <c r="F82">
         <v>25.596930100000002</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B83" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C83" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D83" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E83">
         <v>45.643102599999999</v>
@@ -3258,19 +3503,22 @@
       <c r="F83">
         <v>25.596314700000001</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B84" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C84" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E84">
         <v>44.466068999999997</v>
@@ -3278,19 +3526,22 @@
       <c r="F84">
         <v>26.06765</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B85" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C85" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D85" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E85">
         <v>44.430190000000003</v>
@@ -3298,19 +3549,22 @@
       <c r="F85">
         <v>26.165937</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G85" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B86" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C86" t="s">
         <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E86">
         <v>45.752189100000002</v>
@@ -3318,19 +3572,22 @@
       <c r="F86">
         <v>21.225358</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G86" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B87" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C87" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D87" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E87">
         <v>44.484184999999997</v>
@@ -3338,19 +3595,22 @@
       <c r="F87">
         <v>26.092829999999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B88" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C88" t="s">
         <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E88">
         <v>45.780524800000002</v>
@@ -3358,19 +3618,22 @@
       <c r="F88">
         <v>21.220014500000001</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B89" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C89" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D89" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E89">
         <v>44.456117999999996</v>
@@ -3378,19 +3641,22 @@
       <c r="F89">
         <v>26.097242000000001</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B90" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C90" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D90" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E90">
         <v>47.159374800000002</v>
@@ -3398,19 +3664,22 @@
       <c r="F90">
         <v>27.611538400000001</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B91" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C91" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D91" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E91">
         <v>47.645679000000001</v>
@@ -3418,19 +3687,22 @@
       <c r="F91">
         <v>26.249789</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B92" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C92" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D92" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E92">
         <v>44.126835800000002</v>
@@ -3438,19 +3710,22 @@
       <c r="F92">
         <v>28.615251700000002</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G92" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B93" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C93" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D93" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E93">
         <v>46.765711500000002</v>
@@ -3458,19 +3733,22 @@
       <c r="F93">
         <v>23.551805099999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B94" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C94" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D94" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E94">
         <v>47.799874000000003</v>
@@ -3478,19 +3756,22 @@
       <c r="F94">
         <v>22.874769000000001</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B95" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C95" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D95" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E95">
         <v>47.144554589999998</v>
@@ -3498,19 +3779,22 @@
       <c r="F95">
         <v>27.607835000000001</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G95" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B96" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C96" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D96" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="E96">
         <v>44.509180000000001</v>
@@ -3518,19 +3802,22 @@
       <c r="F96">
         <v>26.089096000000001</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G96" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B97" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C97" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D97" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="E97">
         <v>45.639418999999997</v>
@@ -3538,19 +3825,22 @@
       <c r="F97">
         <v>25.622464000000001</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B98" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C98" t="s">
         <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="E98">
         <v>45.731428000000001</v>
@@ -3558,19 +3848,22 @@
       <c r="F98">
         <v>21.262076199999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B99" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C99" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D99" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E99">
         <v>46.755287699999997</v>
@@ -3578,19 +3871,22 @@
       <c r="F99">
         <v>23.5578243</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G99" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B100" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C100" t="s">
         <v>2</v>
       </c>
       <c r="D100" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="E100">
         <v>45.704279999999997</v>
@@ -3598,19 +3894,22 @@
       <c r="F100">
         <v>21.2166222</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G100" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B101" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C101" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D101" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E101">
         <v>44.480573999999997</v>
@@ -3618,19 +3917,22 @@
       <c r="F101">
         <v>26.115947999999999</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G101" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B102" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C102" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D102" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E102">
         <v>44.428426999999999</v>
@@ -3638,19 +3940,22 @@
       <c r="F102">
         <v>26.105991</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G102" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B103" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C103" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D103" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="E103">
         <v>44.871692000000003</v>
@@ -3658,19 +3963,22 @@
       <c r="F103">
         <v>24.851455000000001</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G103" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B104" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C104" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D104" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E104">
         <v>44.458343999999997</v>
@@ -3678,19 +3986,22 @@
       <c r="F104">
         <v>26.078393999999999</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G104" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B105" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C105" t="s">
         <v>2</v>
       </c>
       <c r="D105" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E105">
         <v>45.740093999999999</v>
@@ -3698,19 +4009,22 @@
       <c r="F105">
         <v>21.225671999999999</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G105" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B106" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C106" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D106" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E106">
         <v>44.484900000000003</v>
@@ -3718,19 +4032,22 @@
       <c r="F106">
         <v>26.033277999999999</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G106" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B107" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C107" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D107" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="E107">
         <v>44.491214999999997</v>
@@ -3738,19 +4055,22 @@
       <c r="F107">
         <v>26.079575999999999</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G107" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B108" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C108" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D108" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E108">
         <v>44.926490999999999</v>
@@ -3758,19 +4078,22 @@
       <c r="F108">
         <v>25.463746</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G108" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B109" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C109" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D109" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E109">
         <v>44.439456</v>
@@ -3778,19 +4101,22 @@
       <c r="F109">
         <v>26.027477999999999</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G109" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B110" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C110" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D110" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="E110">
         <v>44.637483000000003</v>
@@ -3798,19 +4124,22 @@
       <c r="F110">
         <v>22.680416000000001</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G110" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B111" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C111" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D111" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E111">
         <v>44.427948000000001</v>
@@ -3818,19 +4147,22 @@
       <c r="F111">
         <v>26.148299999999999</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G111" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B112" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C112" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D112" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="E112">
         <v>44.601540999999997</v>
@@ -3838,19 +4170,22 @@
       <c r="F112">
         <v>26.070585999999999</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G112" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B113" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C113" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D113" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E113">
         <v>44.420634999999997</v>
@@ -3858,19 +4193,22 @@
       <c r="F113">
         <v>26.164988999999998</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G113" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B114" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C114" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D114" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="E114">
         <v>47.640667000000001</v>
@@ -3878,19 +4216,22 @@
       <c r="F114">
         <v>22.889037999999999</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G114" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B115" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C115" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D115" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E115">
         <v>46.766421999999999</v>
@@ -3898,19 +4239,22 @@
       <c r="F115">
         <v>23.549433000000001</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G115" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B116" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C116" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D116" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E116">
         <v>45.117908</v>
@@ -3918,19 +4262,22 @@
       <c r="F116">
         <v>24.363218</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G116" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B117" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C117" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D117" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E117">
         <v>44.452694999999999</v>
@@ -3938,19 +4285,22 @@
       <c r="F117">
         <v>26.111875999999999</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G117" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B118" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C118" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D118" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E118">
         <v>44.451819</v>
@@ -3958,19 +4308,22 @@
       <c r="F118">
         <v>26.084181999999998</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G118" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B119" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C119" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D119" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E119">
         <v>44.474471000000001</v>
@@ -3978,19 +4331,22 @@
       <c r="F119">
         <v>26.068762</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G119" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B120" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C120" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D120" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E120">
         <v>45.101947000000003</v>
@@ -3998,19 +4354,22 @@
       <c r="F120">
         <v>24.365331999999999</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G120" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B121" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C121" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D121" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E121">
         <v>44.461588999999996</v>
@@ -4018,19 +4377,22 @@
       <c r="F121">
         <v>26.073038</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G121" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B122" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C122" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D122" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E122">
         <v>44.432416000000003</v>
@@ -4038,19 +4400,22 @@
       <c r="F122">
         <v>26.071452000000001</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G122" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B123" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C123" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D123" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E123">
         <v>44.440389000000003</v>
@@ -4058,19 +4423,22 @@
       <c r="F123">
         <v>26.080891000000001</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G123" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B124" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C124" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D124" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E124">
         <v>44.494776000000002</v>
@@ -4078,19 +4446,22 @@
       <c r="F124">
         <v>26.014659000000002</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G124" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B125" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C125" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D125" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E125">
         <v>44.871653999999999</v>
@@ -4098,445 +4469,514 @@
       <c r="F125">
         <v>24.847249000000001</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G125" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B126" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C126" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D126" t="s">
-        <v>366</v>
-      </c>
-      <c r="E126" t="s">
-        <v>367</v>
-      </c>
-      <c r="F126" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+      <c r="E126">
+        <v>44.434429000000002</v>
+      </c>
+      <c r="F126">
+        <v>26.028086999999999</v>
+      </c>
+      <c r="G126" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B127" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C127" t="s">
-        <v>6</v>
+        <v>197</v>
       </c>
       <c r="D127" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E127">
-        <v>44.434429000000002</v>
+        <v>45.686644999999999</v>
       </c>
       <c r="F127">
-        <v>26.028086999999999</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21.907765999999999</v>
+      </c>
+      <c r="G127" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B128" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C128" t="s">
-        <v>195</v>
+        <v>91</v>
       </c>
       <c r="D128" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="E128">
-        <v>45.686644999999999</v>
+        <v>45.66563</v>
       </c>
       <c r="F128">
-        <v>21.907765999999999</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25.599231</v>
+      </c>
+      <c r="G128" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B129" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C129" t="s">
-        <v>89</v>
+        <v>377</v>
       </c>
       <c r="D129" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E129">
-        <v>45.66563</v>
+        <v>44.551228999999999</v>
       </c>
       <c r="F129">
-        <v>25.599231</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26.072780000000002</v>
+      </c>
+      <c r="G129" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B130" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C130" t="s">
-        <v>378</v>
+        <v>97</v>
       </c>
       <c r="D130" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E130">
-        <v>44.551228999999999</v>
+        <v>44.871581999999997</v>
       </c>
       <c r="F130">
-        <v>26.072780000000002</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24.843973999999999</v>
+      </c>
+      <c r="G130" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>380</v>
+      </c>
+      <c r="B131" t="s">
+        <v>381</v>
+      </c>
+      <c r="C131" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131" t="s">
+        <v>381</v>
+      </c>
+      <c r="E131">
+        <v>44.437975999999999</v>
+      </c>
+      <c r="F131">
+        <v>26.135684999999999</v>
+      </c>
+      <c r="G131" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>382</v>
+      </c>
+      <c r="B132" t="s">
         <v>379</v>
       </c>
-      <c r="B131" t="s">
-        <v>380</v>
-      </c>
-      <c r="C131" t="s">
-        <v>95</v>
-      </c>
-      <c r="D131" t="s">
-        <v>380</v>
-      </c>
-      <c r="E131">
-        <v>44.871581999999997</v>
-      </c>
-      <c r="F131">
-        <v>24.843973999999999</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>381</v>
-      </c>
-      <c r="B132" t="s">
-        <v>382</v>
-      </c>
       <c r="C132" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="D132" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E132">
-        <v>44.437975999999999</v>
+        <v>44.844670000000001</v>
       </c>
       <c r="F132">
-        <v>26.135684999999999</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24.881067000000002</v>
+      </c>
+      <c r="G132" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>383</v>
       </c>
       <c r="B133" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="C133" t="s">
-        <v>95</v>
+        <v>165</v>
       </c>
       <c r="D133" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="E133">
-        <v>44.844670000000001</v>
+        <v>43.891616999999997</v>
       </c>
       <c r="F133">
-        <v>24.881067000000002</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25.967739999999999</v>
+      </c>
+      <c r="G133" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B134" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C134" t="s">
-        <v>163</v>
+        <v>53</v>
       </c>
       <c r="D134" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E134">
-        <v>43.891616999999997</v>
+        <v>44.943952000000003</v>
       </c>
       <c r="F134">
-        <v>25.967739999999999</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26.021298000000002</v>
+      </c>
+      <c r="G134" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B135" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C135" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="D135" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E135">
-        <v>44.943952000000003</v>
+        <v>45.092314000000002</v>
       </c>
       <c r="F135">
-        <v>26.021298000000002</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24.371713</v>
+      </c>
+      <c r="G135" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B136" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C136" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D136" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E136">
-        <v>45.092314000000002</v>
+        <v>44.319271000000001</v>
       </c>
       <c r="F136">
-        <v>24.371713</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+        <v>28.603801000000001</v>
+      </c>
+      <c r="G136" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B137" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C137" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="D137" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E137">
-        <v>44.319271000000001</v>
+        <v>44.479779999999998</v>
       </c>
       <c r="F137">
-        <v>28.603801000000001</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26.100037</v>
+      </c>
+      <c r="G137" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B138" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C138" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D138" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E138">
-        <v>44.479779999999998</v>
+        <v>44.420279000000001</v>
       </c>
       <c r="F138">
-        <v>26.100037</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26.018508000000001</v>
+      </c>
+      <c r="G138" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B139" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C139" t="s">
-        <v>6</v>
+        <v>186</v>
       </c>
       <c r="D139" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E139">
-        <v>44.420279000000001</v>
+        <v>44.562693000000003</v>
       </c>
       <c r="F139">
-        <v>26.018508000000001</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27.361305000000002</v>
+      </c>
+      <c r="G139" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B140" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C140" t="s">
-        <v>184</v>
+        <v>7</v>
       </c>
       <c r="D140" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="E140">
-        <v>44.562693000000003</v>
+        <v>44.488191</v>
       </c>
       <c r="F140">
-        <v>27.361305000000002</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26.051618999999999</v>
+      </c>
+      <c r="G140" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B141" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C141" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D141" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E141">
-        <v>44.488191</v>
+        <v>44.516531999999998</v>
       </c>
       <c r="F141">
-        <v>26.051618999999999</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26.013863000000001</v>
+      </c>
+      <c r="G141" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B142" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C142" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D142" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E142">
-        <v>44.516531999999998</v>
+        <v>44.399574000000001</v>
       </c>
       <c r="F142">
-        <v>26.013863000000001</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26.043849999999999</v>
+      </c>
+      <c r="G142" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B143" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C143" t="s">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="D143" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E143">
-        <v>44.399574000000001</v>
-      </c>
-      <c r="F143">
-        <v>26.043849999999999</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+        <v>45.426881999999999</v>
+      </c>
+      <c r="F143" t="s">
+        <v>406</v>
+      </c>
+      <c r="G143" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
+        <v>407</v>
+      </c>
+      <c r="B144" t="s">
+        <v>408</v>
+      </c>
+      <c r="C144" t="s">
+        <v>409</v>
+      </c>
+      <c r="D144" t="s">
+        <v>408</v>
+      </c>
+      <c r="E144">
+        <v>44.199156000000002</v>
+      </c>
+      <c r="F144">
+        <v>27.330266999999999</v>
+      </c>
+      <c r="G144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>410</v>
+      </c>
+      <c r="B145" t="s">
+        <v>411</v>
+      </c>
+      <c r="C145" t="s">
+        <v>7</v>
+      </c>
+      <c r="D145" t="s">
+        <v>411</v>
+      </c>
+      <c r="E145">
+        <v>44.465406000000002</v>
+      </c>
+      <c r="F145">
+        <v>26.066955</v>
+      </c>
+      <c r="G145" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>412</v>
+      </c>
+      <c r="B146" t="s">
+        <v>413</v>
+      </c>
+      <c r="C146" t="s">
+        <v>414</v>
+      </c>
+      <c r="D146" t="s">
+        <v>413</v>
+      </c>
+      <c r="E146">
+        <v>44.688599000000004</v>
+      </c>
+      <c r="F146">
+        <v>26.146923999999999</v>
+      </c>
+      <c r="G146" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
         <v>415</v>
       </c>
-      <c r="B144" t="s">
-        <v>405</v>
-      </c>
-      <c r="C144" t="s">
-        <v>135</v>
-      </c>
-      <c r="D144" t="s">
-        <v>405</v>
-      </c>
-      <c r="E144">
-        <v>45.426881999999999</v>
-      </c>
-      <c r="F144" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>407</v>
-      </c>
-      <c r="B145" t="s">
-        <v>408</v>
-      </c>
-      <c r="C145" t="s">
-        <v>409</v>
-      </c>
-      <c r="D145" t="s">
-        <v>408</v>
-      </c>
-      <c r="E145">
-        <v>44.199156000000002</v>
-      </c>
-      <c r="F145">
-        <v>27.330266999999999</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
-        <v>410</v>
-      </c>
-      <c r="B146" t="s">
-        <v>411</v>
-      </c>
-      <c r="C146" t="s">
-        <v>6</v>
-      </c>
-      <c r="D146" t="s">
-        <v>411</v>
-      </c>
-      <c r="E146">
-        <v>44.465406000000002</v>
-      </c>
-      <c r="F146">
-        <v>26.066955</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>414</v>
-      </c>
       <c r="B147" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="C147" t="s">
-        <v>413</v>
+        <v>7</v>
       </c>
       <c r="D147" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="E147">
-        <v>44.688599000000004</v>
+        <v>44.480876000000002</v>
       </c>
       <c r="F147">
-        <v>26.146923999999999</v>
+        <v>26.117827999999999</v>
+      </c>
+      <c r="G147" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>